<commit_message>
changed the name of the dataset to LG (FAO Land and Gender) and indicators to LG-XXXX
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/FAO-LandAndGender/FAO-LandAndGender.1Fa.xlsx
+++ b/Simple_XLS_Importer/data/FAO-LandAndGender/FAO-LandAndGender.1Fa.xlsx
@@ -467,10 +467,10 @@
     <t>Numeric</t>
   </si>
   <si>
-    <t>LandAndGender</t>
-  </si>
-  <si>
-    <t>LandAndGender.1Fa</t>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>LG.1Fa</t>
   </si>
 </sst>
 </file>

</xml_diff>